<commit_message>
added treatment episodes for altmeds & started on switching script
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/analysis/definitions/bridge/ADEPT_O1_BRIDGE_19Mayo25.xlsx
+++ b/DEVELOPMENT/analysis/definitions/bridge/ADEPT_O1_BRIDGE_19Mayo25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\ADEPT_obj1\DEVELOPMENT\analysis\definitions\bridge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0782EA8-0061-4AF4-9F16-8015CF4EC10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94894432-206D-462E-9E0D-DA2BA39728AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2506CD93-0285-9E44-BBDD-A2C4E77A0341}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALG!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OBJ1'!$A$1:$K$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OBJ1'!$A$1:$K$181</definedName>
   </definedNames>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
@@ -2116,7 +2116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FA1CCF-AC46-4BBB-901E-A0CC50A7045D}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K181"/>
@@ -2175,7 +2175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>65</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>67</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>69</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>71</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>73</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>75</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>77</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>79</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>81</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>83</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>85</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>87</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>89</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>93</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>95</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>97</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>99</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>101</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>103</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>105</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>107</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>109</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>111</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>113</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>115</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>117</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>119</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>121</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>123</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>125</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>127</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>129</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>131</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>133</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>135</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>137</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>139</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>141</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>143</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>145</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>147</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>149</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>151</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>153</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>155</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>165</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
         <v>167</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
         <v>169</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>171</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>173</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>175</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>177</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>179</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>181</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>183</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>187</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>189</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
         <v>191</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>193</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>195</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>197</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>199</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>201</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>203</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>205</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>207</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>209</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>211</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>213</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>215</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>217</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>219</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>221</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>223</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>225</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>227</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>229</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>231</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>233</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>235</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>237</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>239</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>241</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>245</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>247</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>249</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>251</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>253</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>255</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>257</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>259</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>261</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>263</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>265</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>267</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>269</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>271</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>273</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>275</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>277</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>279</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>281</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>283</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>285</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>287</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>289</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>291</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>293</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>85</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>121</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>295</v>
       </c>
@@ -7284,7 +7284,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>297</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>299</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>301</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>303</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>305</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>307</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>309</v>
       </c>
@@ -7559,7 +7559,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>313</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>315</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>325</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>329</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>331</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>333</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>335</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>339</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>341</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="10" t="s">
         <v>343</v>
       </c>
@@ -8089,7 +8089,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>345</v>
       </c>
@@ -8124,7 +8124,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>347</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>349</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>351</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>355</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>357</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>359</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="18" t="s">
         <v>361</v>
       </c>
@@ -8383,7 +8383,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K181" xr:uid="{E0FDDF39-709C-C14C-B461-AFB2AA297754}"/>
+  <autoFilter ref="A1:K181" xr:uid="{E0FDDF39-709C-C14C-B461-AFB2AA297754}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14303,6 +14309,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="70fbc179-56b2-4609-9c4f-f2d8c8a53629">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D26C639087F6D45ADFC3EC21F1D3A6E" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="878129f2fcc6ee12aa7a3f6919ba358e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70fbc179-56b2-4609-9c4f-f2d8c8a53629" xmlns:ns3="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f17d72d02eee5b7172274046075b6715" ns2:_="" ns3:_="">
     <xsd:import namespace="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
@@ -14503,27 +14529,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="70fbc179-56b2-4609-9c4f-f2d8c8a53629">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a1800618-4cc3-44a3-b2ff-4430b6f3c67d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B141F6-1B65-48D6-AC6D-6863CE810BB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{794DD23A-82BD-4D35-84D2-4A4CA4219C4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
+    <ds:schemaRef ds:uri="a1800618-4cc3-44a3-b2ff-4430b6f3c67d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{461DAC6E-9E86-4423-A9B0-363BFCF6664C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14540,23 +14565,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{794DD23A-82BD-4D35-84D2-4A4CA4219C4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="70fbc179-56b2-4609-9c4f-f2d8c8a53629"/>
-    <ds:schemaRef ds:uri="a1800618-4cc3-44a3-b2ff-4430b6f3c67d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B141F6-1B65-48D6-AC6D-6863CE810BB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>